<commit_message>
Fixed an consistency issue with the error codes
</commit_message>
<xml_diff>
--- a/docs/packages/CDVM/test_cases/CDVM Test Cases.xlsx
+++ b/docs/packages/CDVM/test_cases/CDVM Test Cases.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1628" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="316">
   <si>
     <t>Extra Notes</t>
   </si>
@@ -1148,6 +1148,18 @@
   </si>
   <si>
     <t>Blank Calendar Year paramter</t>
+  </si>
+  <si>
+    <t>executing test case (V_FISC_YEAR) for ORA-20525
+The cruises for the specified fiscal year were NOT processed successfully
+ORA-20525: The Cruise Fiscal Year parameter was not specified
+completed test case for ORA-20525</t>
+  </si>
+  <si>
+    <t>executing test case (V_CAL_YEAR) for ORA-20527
+The cruises for the specified calendar year were NOT processed successfully
+ORA-20527: The Cruise Calendar Year parameter was not specified
+completed test case for ORA-20527</t>
   </si>
 </sst>
 </file>
@@ -3791,7 +3803,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4262,27 +4274,31 @@
         <v>-20522</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B28" s="29" t="s">
         <v>309</v>
       </c>
       <c r="C28" s="29" t="s">
         <v>312</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28">
+      <c r="D28" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="E28" s="2">
         <v>-20525</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="B29" s="29" t="s">
         <v>310</v>
       </c>
       <c r="C29" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29">
+      <c r="D29" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="E29" s="2">
         <v>-20527</v>
       </c>
     </row>

</xml_diff>